<commit_message>
fix the templates - hot fix - will implement the computational changes soon
</commit_message>
<xml_diff>
--- a/excel_templates/buildings-template.xlsx
+++ b/excel_templates/buildings-template.xlsx
@@ -12,14 +12,14 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8910"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Name</t>
   </si>
@@ -28,13 +28,28 @@
   </si>
   <si>
     <t>May An Phu</t>
+  </si>
+  <si>
+    <t>Data type</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Text</t>
+  </si>
+  <si>
+    <t>Requirement</t>
+  </si>
+  <si>
+    <t>Compulsory</t>
+  </si>
+  <si>
+    <t>Separate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -48,8 +63,45 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -57,19 +109,25 @@
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
+      <patternFill patternType="lightUp">
+        <fgColor theme="4"/>
+        <bgColor theme="4" tint="-0.24994659260841701"/>
+      </patternFill>
+    </fill>
+    <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -92,26 +150,70 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -392,101 +494,163 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" customWidth="1"/>
+    <col min="4" max="4" width="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
+      <c r="A5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="11"/>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="8"/>
+      <c r="B6" s="9"/>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="B7" s="9"/>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" s="9"/>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="8"/>
+      <c r="B9" s="9"/>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
+      <c r="B10" s="9"/>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11" s="9"/>
+    </row>
+    <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="9"/>
+    </row>
+    <row r="13" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
+      <c r="B13" s="9"/>
+    </row>
+    <row r="14" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="8"/>
+      <c r="B14" s="9"/>
+    </row>
+    <row r="15" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+      <c r="B15" s="9"/>
+    </row>
+    <row r="16" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
+      <c r="B16" s="9"/>
+    </row>
+    <row r="17" spans="1:2" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+      <c r="B17" s="9"/>
+    </row>
+    <row r="18" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
+      <c r="B18" s="9"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="10"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="10"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="10"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="10"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="10"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="10"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="10"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="10"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="10"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="10"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B29" s="10"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B30" s="10"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B31" s="10"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B32" s="10"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="10"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="10"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="10"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A6:A18"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>